<commit_message>
- clustering algorithms experiment has been implemented  - several issues regarding the JavaML library have been fixed
</commit_message>
<xml_diff>
--- a/results/overall.xlsx
+++ b/results/overall.xlsx
@@ -4,20 +4,38 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="13860" windowHeight="6420" activeTab="3"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="13860" windowHeight="6420" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Karate" sheetId="1" r:id="rId1"/>
     <sheet name="Sawmill" sheetId="2" r:id="rId2"/>
     <sheet name="NCAA Football" sheetId="3" r:id="rId3"/>
     <sheet name="Overall" sheetId="5" r:id="rId4"/>
+    <sheet name="Clustering Algorithms" sheetId="6" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="clusterings_compare" localSheetId="4">'Clustering Algorithms'!$A$3:$C$231</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="clusterings_compare" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="852" sourceFile="C:\Users\Lucas\Desktop\SourceCode\datamining-criteria\results\clusterings_compare.txt" decimal="," thousands=" " semicolon="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2101" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2763" uniqueCount="231">
   <si>
     <t>Criteria</t>
   </si>
@@ -110,6 +128,606 @@
   </si>
   <si>
     <t>OVERALL AVERAGE RESULTS</t>
+  </si>
+  <si>
+    <t>###### DATASET: Zahary Karate Dataset - Weightened Undirected. #####</t>
+  </si>
+  <si>
+    <t>For clustering: Jung Bicomponent Clusterer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Jaccard] Jaccard Coefficient External Evaluation: 0.4605089949506484</t>
+  </si>
+  <si>
+    <t>Modularity Q Criteria Calculator</t>
+  </si>
+  <si>
+    <t>Neighbour Overlap Distance Calculator</t>
+  </si>
+  <si>
+    <t>0.10046756994808943</t>
+  </si>
+  <si>
+    <t>Edge Path Distance Calculator</t>
+  </si>
+  <si>
+    <t>Adjacency Relation Distance Calculator</t>
+  </si>
+  <si>
+    <t>Pearson Correlation Distance Calculator</t>
+  </si>
+  <si>
+    <t>C Index Criteria Calculator</t>
+  </si>
+  <si>
+    <t>0.18064609786610283</t>
+  </si>
+  <si>
+    <t>0.916919457375983</t>
+  </si>
+  <si>
+    <t>0.4985120814096288</t>
+  </si>
+  <si>
+    <t>0.2258478458692724</t>
+  </si>
+  <si>
+    <t>Davies Bouldin Criteria Calculator</t>
+  </si>
+  <si>
+    <t>1.1022267881136072</t>
+  </si>
+  <si>
+    <t>Infinity</t>
+  </si>
+  <si>
+    <t>1.4570405169471183</t>
+  </si>
+  <si>
+    <t>0.9654637132956236</t>
+  </si>
+  <si>
+    <t>Silhouette Width Criteria 2 Calculator</t>
+  </si>
+  <si>
+    <t>-0.027344210837022036</t>
+  </si>
+  <si>
+    <t>-0.9399403239556694</t>
+  </si>
+  <si>
+    <t>-0.15745426903474244</t>
+  </si>
+  <si>
+    <t>-0.09474537669292894</t>
+  </si>
+  <si>
+    <t>Variance Ratio Criteria Calculator</t>
+  </si>
+  <si>
+    <t>19.239870629476638</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>3.4789342341615765</t>
+  </si>
+  <si>
+    <t>12.6025350107332</t>
+  </si>
+  <si>
+    <t>PBM Criteria Calculator</t>
+  </si>
+  <si>
+    <t>0.014039332551747304</t>
+  </si>
+  <si>
+    <t>0.016666666666666666</t>
+  </si>
+  <si>
+    <t>0.013773725298722669</t>
+  </si>
+  <si>
+    <t>0.01756247213035195</t>
+  </si>
+  <si>
+    <t>Dunn Index Criteria Calculator</t>
+  </si>
+  <si>
+    <t>0.7574074074074079</t>
+  </si>
+  <si>
+    <t>5.562684646268003E-309</t>
+  </si>
+  <si>
+    <t>0.2548235957188129</t>
+  </si>
+  <si>
+    <t>0.3292723778722483</t>
+  </si>
+  <si>
+    <t>Z-Statistics Criteria Calculator</t>
+  </si>
+  <si>
+    <t>390.23776422909236</t>
+  </si>
+  <si>
+    <t>32.89135968974835</t>
+  </si>
+  <si>
+    <t>316.6988678293565</t>
+  </si>
+  <si>
+    <t>194.52756369360802</t>
+  </si>
+  <si>
+    <t>Point Biserial Criteria Calculator</t>
+  </si>
+  <si>
+    <t>55.63821204182208</t>
+  </si>
+  <si>
+    <t>50.91231568412392</t>
+  </si>
+  <si>
+    <t>59.291096242048255</t>
+  </si>
+  <si>
+    <t>46.487156918183686</t>
+  </si>
+  <si>
+    <t>For clustering: Jung Edge Betweenness Clusterer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Jaccard] Jaccard Coefficient External Evaluation: 0.4866310160427806</t>
+  </si>
+  <si>
+    <t>0.025552369708213844</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.4285714285714287</t>
+  </si>
+  <si>
+    <t>-0.2000000000000001</t>
+  </si>
+  <si>
+    <t>4.9E-324</t>
+  </si>
+  <si>
+    <t>0.029411764705882356</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>1.668805393880401E-308</t>
+  </si>
+  <si>
+    <t>609.0603919263048</t>
+  </si>
+  <si>
+    <t>36.07588943941051</t>
+  </si>
+  <si>
+    <t>479.01752235192373</t>
+  </si>
+  <si>
+    <t>315.0580627947995</t>
+  </si>
+  <si>
+    <t>For clustering: Jung Voltage Clusterer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Jaccard] Jaccard Coefficient External Evaluation: 0.5187105584220729</t>
+  </si>
+  <si>
+    <t>0.12809729952587093</t>
+  </si>
+  <si>
+    <t>0.2475895522660684</t>
+  </si>
+  <si>
+    <t>0.8263149947000463</t>
+  </si>
+  <si>
+    <t>0.43187310694120346</t>
+  </si>
+  <si>
+    <t>0.2789870794384364</t>
+  </si>
+  <si>
+    <t>1.392261098430386</t>
+  </si>
+  <si>
+    <t>2.307484603443498</t>
+  </si>
+  <si>
+    <t>1.1875274297517227</t>
+  </si>
+  <si>
+    <t>-0.004260816262939314</t>
+  </si>
+  <si>
+    <t>-0.7537472707243592</t>
+  </si>
+  <si>
+    <t>-0.008712130142009744</t>
+  </si>
+  <si>
+    <t>-0.024243677206292433</t>
+  </si>
+  <si>
+    <t>28.65923300477113</t>
+  </si>
+  <si>
+    <t>8.274223223783693E-306</t>
+  </si>
+  <si>
+    <t>10.490549192511583</t>
+  </si>
+  <si>
+    <t>28.44695419805719</t>
+  </si>
+  <si>
+    <t>0.019660098204090756</t>
+  </si>
+  <si>
+    <t>3.80249229034177E-309</t>
+  </si>
+  <si>
+    <t>0.013509172937091585</t>
+  </si>
+  <si>
+    <t>0.02323102775825919</t>
+  </si>
+  <si>
+    <t>0.5061823361823361</t>
+  </si>
+  <si>
+    <t>0.15921612870199006</t>
+  </si>
+  <si>
+    <t>0.18740978296128236</t>
+  </si>
+  <si>
+    <t>346.8773762962795</t>
+  </si>
+  <si>
+    <t>29.52579699323996</t>
+  </si>
+  <si>
+    <t>272.93485473967434</t>
+  </si>
+  <si>
+    <t>172.19629018537836</t>
+  </si>
+  <si>
+    <t>29.00668096788241</t>
+  </si>
+  <si>
+    <t>40.113261178543624</t>
+  </si>
+  <si>
+    <t>27.75077753608798</t>
+  </si>
+  <si>
+    <t>20.57098804580455</t>
+  </si>
+  <si>
+    <t>For clustering: JavaML Density Based Spatial Clustering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Jaccard] Jaccard Coefficient External Evaluation: 0.4526717087868168</t>
+  </si>
+  <si>
+    <t>0.021675221126581313</t>
+  </si>
+  <si>
+    <t>0.262039093595844</t>
+  </si>
+  <si>
+    <t>0.8492958328170821</t>
+  </si>
+  <si>
+    <t>0.558564512088685</t>
+  </si>
+  <si>
+    <t>0.3547832539308114</t>
+  </si>
+  <si>
+    <t>1.1127941772401195</t>
+  </si>
+  <si>
+    <t>1.2980264106305408</t>
+  </si>
+  <si>
+    <t>0.8386866098842202</t>
+  </si>
+  <si>
+    <t>-0.016609213100506857</t>
+  </si>
+  <si>
+    <t>-0.7273075301279422</t>
+  </si>
+  <si>
+    <t>-0.03514983343082651</t>
+  </si>
+  <si>
+    <t>-0.04840170272804344</t>
+  </si>
+  <si>
+    <t>5.0978434527518806</t>
+  </si>
+  <si>
+    <t>5.81683752699527E-306</t>
+  </si>
+  <si>
+    <t>4.234576743879832</t>
+  </si>
+  <si>
+    <t>5.696712179536347</t>
+  </si>
+  <si>
+    <t>0.019614075103632243</t>
+  </si>
+  <si>
+    <t>1.650263111726175E-309</t>
+  </si>
+  <si>
+    <t>0.017460327313029173</t>
+  </si>
+  <si>
+    <t>0.023525812774654476</t>
+  </si>
+  <si>
+    <t>0.6032223871104515</t>
+  </si>
+  <si>
+    <t>9.3947562914749E-310</t>
+  </si>
+  <si>
+    <t>0.24376003116884168</t>
+  </si>
+  <si>
+    <t>0.21459624380632653</t>
+  </si>
+  <si>
+    <t>503.46955871547294</t>
+  </si>
+  <si>
+    <t>27.83821941138085</t>
+  </si>
+  <si>
+    <t>411.2798888028743</t>
+  </si>
+  <si>
+    <t>277.5012953846243</t>
+  </si>
+  <si>
+    <t>85.09624107865456</t>
+  </si>
+  <si>
+    <t>32.721512240961836</t>
+  </si>
+  <si>
+    <t>81.6617565661445</t>
+  </si>
+  <si>
+    <t>82.78286251258804</t>
+  </si>
+  <si>
+    <t>For clustering: JavaML KNode Clustering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Jaccard] Jaccard Coefficient External Evaluation: 0.495616880650531</t>
+  </si>
+  <si>
+    <t>0.03703325880534378</t>
+  </si>
+  <si>
+    <t>0.16444965781240056</t>
+  </si>
+  <si>
+    <t>0.5844549976285407</t>
+  </si>
+  <si>
+    <t>0.13367560477810442</t>
+  </si>
+  <si>
+    <t>0.19711628953958574</t>
+  </si>
+  <si>
+    <t>1.1335422983649406</t>
+  </si>
+  <si>
+    <t>1.049729747166226</t>
+  </si>
+  <si>
+    <t>0.9536897948681037</t>
+  </si>
+  <si>
+    <t>-0.004485760022268611</t>
+  </si>
+  <si>
+    <t>-0.4214964398268393</t>
+  </si>
+  <si>
+    <t>0.007091764324836521</t>
+  </si>
+  <si>
+    <t>-0.011291886027816427</t>
+  </si>
+  <si>
+    <t>5.963973383298846</t>
+  </si>
+  <si>
+    <t>3.8400000000000003</t>
+  </si>
+  <si>
+    <t>5.849053892822862</t>
+  </si>
+  <si>
+    <t>7.24247488735247</t>
+  </si>
+  <si>
+    <t>0.01903750785850099</t>
+  </si>
+  <si>
+    <t>4.406110624662539E305</t>
+  </si>
+  <si>
+    <t>0.030778091073152398</t>
+  </si>
+  <si>
+    <t>0.02329879384851664</t>
+  </si>
+  <si>
+    <t>0.63421199445618</t>
+  </si>
+  <si>
+    <t>1.020708484299335E-309</t>
+  </si>
+  <si>
+    <t>0.4724121677126524</t>
+  </si>
+  <si>
+    <t>0.36767879767031264</t>
+  </si>
+  <si>
+    <t>505.3776222990005</t>
+  </si>
+  <si>
+    <t>20.73916072443412</t>
+  </si>
+  <si>
+    <t>373.87650297977484</t>
+  </si>
+  <si>
+    <t>272.46424185337514</t>
+  </si>
+  <si>
+    <t>72.45628572158397</t>
+  </si>
+  <si>
+    <t>10.995626375615204</t>
+  </si>
+  <si>
+    <t>51.594122637732426</t>
+  </si>
+  <si>
+    <t>65.78926192806186</t>
+  </si>
+  <si>
+    <t>For clustering: JavaML Self Organizing Maps Clustering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [Jaccard] Jaccard Coefficient External Evaluation: 0.6724051154863459</t>
+  </si>
+  <si>
+    <t>0.14105094518991249</t>
+  </si>
+  <si>
+    <t>0.22555020106813498</t>
+  </si>
+  <si>
+    <t>0.6250526576632385</t>
+  </si>
+  <si>
+    <t>0.3239879888281027</t>
+  </si>
+  <si>
+    <t>0.24271250242535564</t>
+  </si>
+  <si>
+    <t>1.4269828253455654</t>
+  </si>
+  <si>
+    <t>2.796286048908365</t>
+  </si>
+  <si>
+    <t>2.5186522430574736</t>
+  </si>
+  <si>
+    <t>-0.008997308056958845</t>
+  </si>
+  <si>
+    <t>-0.6793731631175604</t>
+  </si>
+  <si>
+    <t>-0.07055159848826993</t>
+  </si>
+  <si>
+    <t>-0.03648795844706942</t>
+  </si>
+  <si>
+    <t>15.23164284430627</t>
+  </si>
+  <si>
+    <t>1.9887006968390017E-306</t>
+  </si>
+  <si>
+    <t>8.649157608140422</t>
+  </si>
+  <si>
+    <t>18.621652270917544</t>
+  </si>
+  <si>
+    <t>0.016728882461919194</t>
+  </si>
+  <si>
+    <t>0.057726063829787226</t>
+  </si>
+  <si>
+    <t>0.012264561334440144</t>
+  </si>
+  <si>
+    <t>0.02157046392335171</t>
+  </si>
+  <si>
+    <t>0.7024086106047137</t>
+  </si>
+  <si>
+    <t>1.140791835393377E-309</t>
+  </si>
+  <si>
+    <t>0.23328003635899983</t>
+  </si>
+  <si>
+    <t>0.3995453059532888</t>
+  </si>
+  <si>
+    <t>271.73976122845016</t>
+  </si>
+  <si>
+    <t>19.88964268316983</t>
+  </si>
+  <si>
+    <t>203.26084429280385</t>
+  </si>
+  <si>
+    <t>138.698551214181</t>
+  </si>
+  <si>
+    <t>-13.363267709961429</t>
+  </si>
+  <si>
+    <t>15.161422543982209</t>
+  </si>
+  <si>
+    <t>-23.032266645955286</t>
+  </si>
+  <si>
+    <t>-23.69162105436469</t>
+  </si>
+  <si>
+    <t>CLUSTERING ALGORITHMS COMPARE</t>
   </si>
 </sst>
 </file>
@@ -189,6 +807,10 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="clusterings_compare" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8245,8 +8867,8 @@
   <sheetPr codeName="Arkusz3"/>
   <dimension ref="A1:S184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -13600,13 +14222,12 @@
     <sortCondition descending="1" ref="D43"/>
   </sortState>
   <mergeCells count="24">
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="R40:S40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:I41"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
@@ -13616,16 +14237,2483 @@
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="R2:S2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="R40:S40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H40:I40"/>
     <mergeCell ref="N40:O40"/>
     <mergeCell ref="P40:Q40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C231"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="63.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>45</v>
+      </c>
+      <c r="B54" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" t="s">
+        <v>35</v>
+      </c>
+      <c r="C56" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>50</v>
+      </c>
+      <c r="B57" t="s">
+        <v>37</v>
+      </c>
+      <c r="C57" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>50</v>
+      </c>
+      <c r="B58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>50</v>
+      </c>
+      <c r="B59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C59" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>55</v>
+      </c>
+      <c r="B60" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>55</v>
+      </c>
+      <c r="B61" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>55</v>
+      </c>
+      <c r="B62" t="s">
+        <v>38</v>
+      </c>
+      <c r="C62" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>55</v>
+      </c>
+      <c r="B63" t="s">
+        <v>39</v>
+      </c>
+      <c r="C63" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65" t="s">
+        <v>37</v>
+      </c>
+      <c r="C65" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66" t="s">
+        <v>38</v>
+      </c>
+      <c r="C66" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>60</v>
+      </c>
+      <c r="B67" t="s">
+        <v>39</v>
+      </c>
+      <c r="C67" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68" t="s">
+        <v>35</v>
+      </c>
+      <c r="C68" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>65</v>
+      </c>
+      <c r="B69" t="s">
+        <v>37</v>
+      </c>
+      <c r="C69" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>65</v>
+      </c>
+      <c r="B70" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>65</v>
+      </c>
+      <c r="B71" t="s">
+        <v>39</v>
+      </c>
+      <c r="C71" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>35</v>
+      </c>
+      <c r="C72" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>70</v>
+      </c>
+      <c r="B73" t="s">
+        <v>37</v>
+      </c>
+      <c r="C73" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>70</v>
+      </c>
+      <c r="B74" t="s">
+        <v>38</v>
+      </c>
+      <c r="C74" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>70</v>
+      </c>
+      <c r="B75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C75" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>35</v>
+      </c>
+      <c r="C76" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>37</v>
+      </c>
+      <c r="C77" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>75</v>
+      </c>
+      <c r="B78" t="s">
+        <v>38</v>
+      </c>
+      <c r="C78" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>75</v>
+      </c>
+      <c r="B79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C79" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>34</v>
+      </c>
+      <c r="B82" t="s">
+        <v>35</v>
+      </c>
+      <c r="C82" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>34</v>
+      </c>
+      <c r="B83" t="s">
+        <v>37</v>
+      </c>
+      <c r="C83" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>34</v>
+      </c>
+      <c r="B84" t="s">
+        <v>38</v>
+      </c>
+      <c r="C84" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>34</v>
+      </c>
+      <c r="B85" t="s">
+        <v>39</v>
+      </c>
+      <c r="C85" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>40</v>
+      </c>
+      <c r="B86" t="s">
+        <v>35</v>
+      </c>
+      <c r="C86" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>40</v>
+      </c>
+      <c r="B87" t="s">
+        <v>37</v>
+      </c>
+      <c r="C87" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>40</v>
+      </c>
+      <c r="B88" t="s">
+        <v>38</v>
+      </c>
+      <c r="C88" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>40</v>
+      </c>
+      <c r="B89" t="s">
+        <v>39</v>
+      </c>
+      <c r="C89" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>45</v>
+      </c>
+      <c r="B90" t="s">
+        <v>35</v>
+      </c>
+      <c r="C90" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>45</v>
+      </c>
+      <c r="B91" t="s">
+        <v>37</v>
+      </c>
+      <c r="C91" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>45</v>
+      </c>
+      <c r="B92" t="s">
+        <v>38</v>
+      </c>
+      <c r="C92" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>45</v>
+      </c>
+      <c r="B93" t="s">
+        <v>39</v>
+      </c>
+      <c r="C93" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>50</v>
+      </c>
+      <c r="B94" t="s">
+        <v>35</v>
+      </c>
+      <c r="C94" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>50</v>
+      </c>
+      <c r="B95" t="s">
+        <v>37</v>
+      </c>
+      <c r="C95" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>50</v>
+      </c>
+      <c r="B96" t="s">
+        <v>38</v>
+      </c>
+      <c r="C96" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>50</v>
+      </c>
+      <c r="B97" t="s">
+        <v>39</v>
+      </c>
+      <c r="C97" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>55</v>
+      </c>
+      <c r="B98" t="s">
+        <v>35</v>
+      </c>
+      <c r="C98" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>55</v>
+      </c>
+      <c r="B99" t="s">
+        <v>37</v>
+      </c>
+      <c r="C99" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>55</v>
+      </c>
+      <c r="B100" t="s">
+        <v>38</v>
+      </c>
+      <c r="C100" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>55</v>
+      </c>
+      <c r="B101" t="s">
+        <v>39</v>
+      </c>
+      <c r="C101" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>60</v>
+      </c>
+      <c r="B102" t="s">
+        <v>35</v>
+      </c>
+      <c r="C102" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>60</v>
+      </c>
+      <c r="B103" t="s">
+        <v>37</v>
+      </c>
+      <c r="C103" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>60</v>
+      </c>
+      <c r="B104" t="s">
+        <v>38</v>
+      </c>
+      <c r="C104" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>60</v>
+      </c>
+      <c r="B105" t="s">
+        <v>39</v>
+      </c>
+      <c r="C105" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>65</v>
+      </c>
+      <c r="B106" t="s">
+        <v>35</v>
+      </c>
+      <c r="C106" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>65</v>
+      </c>
+      <c r="B107" t="s">
+        <v>37</v>
+      </c>
+      <c r="C107" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>65</v>
+      </c>
+      <c r="B108" t="s">
+        <v>38</v>
+      </c>
+      <c r="C108" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>65</v>
+      </c>
+      <c r="B109" t="s">
+        <v>39</v>
+      </c>
+      <c r="C109" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>70</v>
+      </c>
+      <c r="B110" t="s">
+        <v>35</v>
+      </c>
+      <c r="C110" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>70</v>
+      </c>
+      <c r="B111" t="s">
+        <v>37</v>
+      </c>
+      <c r="C111" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>70</v>
+      </c>
+      <c r="B112" t="s">
+        <v>38</v>
+      </c>
+      <c r="C112" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>70</v>
+      </c>
+      <c r="B113" t="s">
+        <v>39</v>
+      </c>
+      <c r="C113" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>75</v>
+      </c>
+      <c r="B114" t="s">
+        <v>35</v>
+      </c>
+      <c r="C114" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>75</v>
+      </c>
+      <c r="B115" t="s">
+        <v>37</v>
+      </c>
+      <c r="C115" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>75</v>
+      </c>
+      <c r="B116" t="s">
+        <v>38</v>
+      </c>
+      <c r="C116" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>75</v>
+      </c>
+      <c r="B117" t="s">
+        <v>39</v>
+      </c>
+      <c r="C117" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
+        <v>34</v>
+      </c>
+      <c r="B120" t="s">
+        <v>35</v>
+      </c>
+      <c r="C120" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>34</v>
+      </c>
+      <c r="B121" t="s">
+        <v>37</v>
+      </c>
+      <c r="C121" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
+        <v>34</v>
+      </c>
+      <c r="B122" t="s">
+        <v>38</v>
+      </c>
+      <c r="C122" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" t="s">
+        <v>34</v>
+      </c>
+      <c r="B123" t="s">
+        <v>39</v>
+      </c>
+      <c r="C123" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
+        <v>40</v>
+      </c>
+      <c r="B124" t="s">
+        <v>35</v>
+      </c>
+      <c r="C124" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>40</v>
+      </c>
+      <c r="B125" t="s">
+        <v>37</v>
+      </c>
+      <c r="C125" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
+        <v>40</v>
+      </c>
+      <c r="B126" t="s">
+        <v>38</v>
+      </c>
+      <c r="C126" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
+        <v>40</v>
+      </c>
+      <c r="B127" t="s">
+        <v>39</v>
+      </c>
+      <c r="C127" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
+        <v>45</v>
+      </c>
+      <c r="B128" t="s">
+        <v>35</v>
+      </c>
+      <c r="C128" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" t="s">
+        <v>45</v>
+      </c>
+      <c r="B129" t="s">
+        <v>37</v>
+      </c>
+      <c r="C129" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" t="s">
+        <v>45</v>
+      </c>
+      <c r="B130" t="s">
+        <v>38</v>
+      </c>
+      <c r="C130" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" t="s">
+        <v>45</v>
+      </c>
+      <c r="B131" t="s">
+        <v>39</v>
+      </c>
+      <c r="C131" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" t="s">
+        <v>50</v>
+      </c>
+      <c r="B132" t="s">
+        <v>35</v>
+      </c>
+      <c r="C132" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" t="s">
+        <v>50</v>
+      </c>
+      <c r="B133" t="s">
+        <v>37</v>
+      </c>
+      <c r="C133" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" t="s">
+        <v>50</v>
+      </c>
+      <c r="B134" t="s">
+        <v>38</v>
+      </c>
+      <c r="C134" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" t="s">
+        <v>50</v>
+      </c>
+      <c r="B135" t="s">
+        <v>39</v>
+      </c>
+      <c r="C135" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" t="s">
+        <v>55</v>
+      </c>
+      <c r="B136" t="s">
+        <v>35</v>
+      </c>
+      <c r="C136" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" t="s">
+        <v>55</v>
+      </c>
+      <c r="B137" t="s">
+        <v>37</v>
+      </c>
+      <c r="C137" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" t="s">
+        <v>55</v>
+      </c>
+      <c r="B138" t="s">
+        <v>38</v>
+      </c>
+      <c r="C138" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" t="s">
+        <v>55</v>
+      </c>
+      <c r="B139" t="s">
+        <v>39</v>
+      </c>
+      <c r="C139" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" t="s">
+        <v>60</v>
+      </c>
+      <c r="B140" t="s">
+        <v>35</v>
+      </c>
+      <c r="C140" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" t="s">
+        <v>60</v>
+      </c>
+      <c r="B141" t="s">
+        <v>37</v>
+      </c>
+      <c r="C141" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" t="s">
+        <v>60</v>
+      </c>
+      <c r="B142" t="s">
+        <v>38</v>
+      </c>
+      <c r="C142" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" t="s">
+        <v>60</v>
+      </c>
+      <c r="B143" t="s">
+        <v>39</v>
+      </c>
+      <c r="C143" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" t="s">
+        <v>65</v>
+      </c>
+      <c r="B144" t="s">
+        <v>35</v>
+      </c>
+      <c r="C144" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" t="s">
+        <v>65</v>
+      </c>
+      <c r="B145" t="s">
+        <v>37</v>
+      </c>
+      <c r="C145" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" t="s">
+        <v>65</v>
+      </c>
+      <c r="B146" t="s">
+        <v>38</v>
+      </c>
+      <c r="C146" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" t="s">
+        <v>65</v>
+      </c>
+      <c r="B147" t="s">
+        <v>39</v>
+      </c>
+      <c r="C147" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" t="s">
+        <v>70</v>
+      </c>
+      <c r="B148" t="s">
+        <v>35</v>
+      </c>
+      <c r="C148" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" t="s">
+        <v>70</v>
+      </c>
+      <c r="B149" t="s">
+        <v>37</v>
+      </c>
+      <c r="C149" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" t="s">
+        <v>70</v>
+      </c>
+      <c r="B150" t="s">
+        <v>38</v>
+      </c>
+      <c r="C150" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" t="s">
+        <v>70</v>
+      </c>
+      <c r="B151" t="s">
+        <v>39</v>
+      </c>
+      <c r="C151" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" t="s">
+        <v>75</v>
+      </c>
+      <c r="B152" t="s">
+        <v>35</v>
+      </c>
+      <c r="C152" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" t="s">
+        <v>75</v>
+      </c>
+      <c r="B153" t="s">
+        <v>37</v>
+      </c>
+      <c r="C153" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" t="s">
+        <v>75</v>
+      </c>
+      <c r="B154" t="s">
+        <v>38</v>
+      </c>
+      <c r="C154" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" t="s">
+        <v>75</v>
+      </c>
+      <c r="B155" t="s">
+        <v>39</v>
+      </c>
+      <c r="C155" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" t="s">
+        <v>34</v>
+      </c>
+      <c r="B158" t="s">
+        <v>35</v>
+      </c>
+      <c r="C158" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" t="s">
+        <v>34</v>
+      </c>
+      <c r="B159" t="s">
+        <v>37</v>
+      </c>
+      <c r="C159" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" t="s">
+        <v>34</v>
+      </c>
+      <c r="B160" t="s">
+        <v>38</v>
+      </c>
+      <c r="C160" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" t="s">
+        <v>34</v>
+      </c>
+      <c r="B161" t="s">
+        <v>39</v>
+      </c>
+      <c r="C161" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" t="s">
+        <v>40</v>
+      </c>
+      <c r="B162" t="s">
+        <v>35</v>
+      </c>
+      <c r="C162" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" t="s">
+        <v>40</v>
+      </c>
+      <c r="B163" t="s">
+        <v>37</v>
+      </c>
+      <c r="C163" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" t="s">
+        <v>40</v>
+      </c>
+      <c r="B164" t="s">
+        <v>38</v>
+      </c>
+      <c r="C164" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" t="s">
+        <v>40</v>
+      </c>
+      <c r="B165" t="s">
+        <v>39</v>
+      </c>
+      <c r="C165" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" t="s">
+        <v>45</v>
+      </c>
+      <c r="B166" t="s">
+        <v>35</v>
+      </c>
+      <c r="C166" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" t="s">
+        <v>45</v>
+      </c>
+      <c r="B167" t="s">
+        <v>37</v>
+      </c>
+      <c r="C167" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" t="s">
+        <v>45</v>
+      </c>
+      <c r="B168" t="s">
+        <v>38</v>
+      </c>
+      <c r="C168" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" t="s">
+        <v>45</v>
+      </c>
+      <c r="B169" t="s">
+        <v>39</v>
+      </c>
+      <c r="C169" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" t="s">
+        <v>50</v>
+      </c>
+      <c r="B170" t="s">
+        <v>35</v>
+      </c>
+      <c r="C170" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" t="s">
+        <v>50</v>
+      </c>
+      <c r="B171" t="s">
+        <v>37</v>
+      </c>
+      <c r="C171" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" t="s">
+        <v>50</v>
+      </c>
+      <c r="B172" t="s">
+        <v>38</v>
+      </c>
+      <c r="C172" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" t="s">
+        <v>50</v>
+      </c>
+      <c r="B173" t="s">
+        <v>39</v>
+      </c>
+      <c r="C173" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" t="s">
+        <v>55</v>
+      </c>
+      <c r="B174" t="s">
+        <v>35</v>
+      </c>
+      <c r="C174" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175" t="s">
+        <v>55</v>
+      </c>
+      <c r="B175" t="s">
+        <v>37</v>
+      </c>
+      <c r="C175" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" t="s">
+        <v>55</v>
+      </c>
+      <c r="B176" t="s">
+        <v>38</v>
+      </c>
+      <c r="C176" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" t="s">
+        <v>55</v>
+      </c>
+      <c r="B177" t="s">
+        <v>39</v>
+      </c>
+      <c r="C177" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" t="s">
+        <v>60</v>
+      </c>
+      <c r="B178" t="s">
+        <v>35</v>
+      </c>
+      <c r="C178" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" t="s">
+        <v>60</v>
+      </c>
+      <c r="B179" t="s">
+        <v>37</v>
+      </c>
+      <c r="C179" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" t="s">
+        <v>60</v>
+      </c>
+      <c r="B180" t="s">
+        <v>38</v>
+      </c>
+      <c r="C180" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" t="s">
+        <v>60</v>
+      </c>
+      <c r="B181" t="s">
+        <v>39</v>
+      </c>
+      <c r="C181" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" t="s">
+        <v>65</v>
+      </c>
+      <c r="B182" t="s">
+        <v>35</v>
+      </c>
+      <c r="C182" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" t="s">
+        <v>65</v>
+      </c>
+      <c r="B183" t="s">
+        <v>37</v>
+      </c>
+      <c r="C183" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" t="s">
+        <v>65</v>
+      </c>
+      <c r="B184" t="s">
+        <v>38</v>
+      </c>
+      <c r="C184" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" t="s">
+        <v>65</v>
+      </c>
+      <c r="B185" t="s">
+        <v>39</v>
+      </c>
+      <c r="C185" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" t="s">
+        <v>70</v>
+      </c>
+      <c r="B186" t="s">
+        <v>35</v>
+      </c>
+      <c r="C186" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" t="s">
+        <v>70</v>
+      </c>
+      <c r="B187" t="s">
+        <v>37</v>
+      </c>
+      <c r="C187" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" t="s">
+        <v>70</v>
+      </c>
+      <c r="B188" t="s">
+        <v>38</v>
+      </c>
+      <c r="C188" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" t="s">
+        <v>70</v>
+      </c>
+      <c r="B189" t="s">
+        <v>39</v>
+      </c>
+      <c r="C189" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" t="s">
+        <v>75</v>
+      </c>
+      <c r="B190" t="s">
+        <v>35</v>
+      </c>
+      <c r="C190" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" t="s">
+        <v>75</v>
+      </c>
+      <c r="B191" t="s">
+        <v>37</v>
+      </c>
+      <c r="C191" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" t="s">
+        <v>75</v>
+      </c>
+      <c r="B192" t="s">
+        <v>38</v>
+      </c>
+      <c r="C192" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" t="s">
+        <v>75</v>
+      </c>
+      <c r="B193" t="s">
+        <v>39</v>
+      </c>
+      <c r="C193" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196" t="s">
+        <v>34</v>
+      </c>
+      <c r="B196" t="s">
+        <v>35</v>
+      </c>
+      <c r="C196" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" t="s">
+        <v>34</v>
+      </c>
+      <c r="B197" t="s">
+        <v>37</v>
+      </c>
+      <c r="C197" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" t="s">
+        <v>34</v>
+      </c>
+      <c r="B198" t="s">
+        <v>38</v>
+      </c>
+      <c r="C198" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" t="s">
+        <v>34</v>
+      </c>
+      <c r="B199" t="s">
+        <v>39</v>
+      </c>
+      <c r="C199" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" t="s">
+        <v>40</v>
+      </c>
+      <c r="B200" t="s">
+        <v>35</v>
+      </c>
+      <c r="C200" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" t="s">
+        <v>40</v>
+      </c>
+      <c r="B201" t="s">
+        <v>37</v>
+      </c>
+      <c r="C201" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" t="s">
+        <v>40</v>
+      </c>
+      <c r="B202" t="s">
+        <v>38</v>
+      </c>
+      <c r="C202" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" t="s">
+        <v>40</v>
+      </c>
+      <c r="B203" t="s">
+        <v>39</v>
+      </c>
+      <c r="C203" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" t="s">
+        <v>45</v>
+      </c>
+      <c r="B204" t="s">
+        <v>35</v>
+      </c>
+      <c r="C204" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" t="s">
+        <v>45</v>
+      </c>
+      <c r="B205" t="s">
+        <v>37</v>
+      </c>
+      <c r="C205" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" t="s">
+        <v>45</v>
+      </c>
+      <c r="B206" t="s">
+        <v>38</v>
+      </c>
+      <c r="C206" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" t="s">
+        <v>45</v>
+      </c>
+      <c r="B207" t="s">
+        <v>39</v>
+      </c>
+      <c r="C207" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" t="s">
+        <v>50</v>
+      </c>
+      <c r="B208" t="s">
+        <v>35</v>
+      </c>
+      <c r="C208" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" t="s">
+        <v>50</v>
+      </c>
+      <c r="B209" t="s">
+        <v>37</v>
+      </c>
+      <c r="C209" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" t="s">
+        <v>50</v>
+      </c>
+      <c r="B210" t="s">
+        <v>38</v>
+      </c>
+      <c r="C210" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" t="s">
+        <v>50</v>
+      </c>
+      <c r="B211" t="s">
+        <v>39</v>
+      </c>
+      <c r="C211" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212" t="s">
+        <v>55</v>
+      </c>
+      <c r="B212" t="s">
+        <v>35</v>
+      </c>
+      <c r="C212" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213" t="s">
+        <v>55</v>
+      </c>
+      <c r="B213" t="s">
+        <v>37</v>
+      </c>
+      <c r="C213" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214" t="s">
+        <v>55</v>
+      </c>
+      <c r="B214" t="s">
+        <v>38</v>
+      </c>
+      <c r="C214" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215" t="s">
+        <v>55</v>
+      </c>
+      <c r="B215" t="s">
+        <v>39</v>
+      </c>
+      <c r="C215" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216" t="s">
+        <v>60</v>
+      </c>
+      <c r="B216" t="s">
+        <v>35</v>
+      </c>
+      <c r="C216" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" t="s">
+        <v>60</v>
+      </c>
+      <c r="B217" t="s">
+        <v>37</v>
+      </c>
+      <c r="C217" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" t="s">
+        <v>60</v>
+      </c>
+      <c r="B218" t="s">
+        <v>38</v>
+      </c>
+      <c r="C218" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" t="s">
+        <v>60</v>
+      </c>
+      <c r="B219" t="s">
+        <v>39</v>
+      </c>
+      <c r="C219" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" t="s">
+        <v>65</v>
+      </c>
+      <c r="B220" t="s">
+        <v>35</v>
+      </c>
+      <c r="C220" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" t="s">
+        <v>65</v>
+      </c>
+      <c r="B221" t="s">
+        <v>37</v>
+      </c>
+      <c r="C221" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222" t="s">
+        <v>65</v>
+      </c>
+      <c r="B222" t="s">
+        <v>38</v>
+      </c>
+      <c r="C222" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" t="s">
+        <v>65</v>
+      </c>
+      <c r="B223" t="s">
+        <v>39</v>
+      </c>
+      <c r="C223" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224" t="s">
+        <v>70</v>
+      </c>
+      <c r="B224" t="s">
+        <v>35</v>
+      </c>
+      <c r="C224" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
+      <c r="A225" t="s">
+        <v>70</v>
+      </c>
+      <c r="B225" t="s">
+        <v>37</v>
+      </c>
+      <c r="C225" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226" t="s">
+        <v>70</v>
+      </c>
+      <c r="B226" t="s">
+        <v>38</v>
+      </c>
+      <c r="C226" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3">
+      <c r="A227" t="s">
+        <v>70</v>
+      </c>
+      <c r="B227" t="s">
+        <v>39</v>
+      </c>
+      <c r="C227" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228" t="s">
+        <v>75</v>
+      </c>
+      <c r="B228" t="s">
+        <v>35</v>
+      </c>
+      <c r="C228" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
+      <c r="A229" t="s">
+        <v>75</v>
+      </c>
+      <c r="B229" t="s">
+        <v>37</v>
+      </c>
+      <c r="C229" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230" t="s">
+        <v>75</v>
+      </c>
+      <c r="B230" t="s">
+        <v>38</v>
+      </c>
+      <c r="C230" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231" t="s">
+        <v>75</v>
+      </c>
+      <c r="B231" t="s">
+        <v>39</v>
+      </c>
+      <c r="C231" t="s">
+        <v>229</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>